<commit_message>
kelas, kelas mhs, ruangan, dan perbaikan
</commit_message>
<xml_diff>
--- a/public/sheets/ex-dsn.xlsx
+++ b/public/sheets/ex-dsn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8044C05-8EC4-4850-8101-09AEF3376D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB25515-9882-46CB-AAB5-2316DB091DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{9546A9C4-5F83-4C6A-84A7-F469CB5B53E8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Bandung</t>
   </si>
@@ -39,18 +39,6 @@
     <t>Jl. Bandung</t>
   </si>
   <si>
-    <t>089237812378</t>
-  </si>
-  <si>
-    <t>089237812379</t>
-  </si>
-  <si>
-    <t>089237812380</t>
-  </si>
-  <si>
-    <t>089237812381</t>
-  </si>
-  <si>
     <t>2000-10-01</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>tatiernawati@poltekedc.ac.id</t>
   </si>
   <si>
-    <t>089237812377</t>
-  </si>
-  <si>
     <t>0003107901</t>
   </si>
   <si>
@@ -172,6 +157,24 @@
   </si>
   <si>
     <t>0003107906</t>
+  </si>
+  <si>
+    <t>0003107907</t>
+  </si>
+  <si>
+    <t>3217023989012396</t>
+  </si>
+  <si>
+    <t>197910032005012007</t>
+  </si>
+  <si>
+    <t>Ade Yuliana, M.T.</t>
+  </si>
+  <si>
+    <t>2000-10-06</t>
+  </si>
+  <si>
+    <t>adeYul@poltekedc.ac.id</t>
   </si>
 </sst>
 </file>
@@ -296,6 +299,275 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC0D696-FF90-4DA4-AB6A-533C2D56DA37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12658725" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Keterangan:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>row[0]              |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>row[1]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                                 |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>row[2]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                                 |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>row[3]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                                                 |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>row[4]     |row[5]         |row[6]|row[7]                                         |row[8]                  |row[9]    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> |row[10]|row[11]|row[12]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NIDN</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                |</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NIK	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>               |NIP		    |Nama                                                   |TP_L        |TG_L            |Agama|Email	                                  |No_Hp	        |Alamat     |pd_id    |Status   |Gender</a:t>
+          </a:r>
+          <a:endParaRPr lang="id-ID">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,24 +867,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D1C5FD-8637-4C3E-8DA1-E8C50D539031}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -620,113 +892,113 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="I1" s="1">
+        <v>89237812378</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K1" s="3">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="I2" s="1">
+        <v>89237812377</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K2" s="3">
         <v>10</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="I3" s="1">
+        <v>89237812379</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>1</v>
@@ -735,39 +1007,39 @@
         <v>10</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <v>89237812380</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>1</v>
@@ -776,39 +1048,39 @@
         <v>10</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>89237812381</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>1</v>
@@ -817,39 +1089,39 @@
         <v>10</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
+      </c>
+      <c r="I6" s="1">
+        <v>89237812382</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>1</v>
@@ -858,10 +1130,51 @@
         <v>10</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1">
+        <v>89237812383</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>10</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -874,8 +1187,10 @@
     <hyperlink ref="H5" r:id="rId5" xr:uid="{70B57B6E-C798-43C5-909A-1D3F26ED0ED7}"/>
     <hyperlink ref="H6" r:id="rId6" xr:uid="{77CF7436-2E68-4747-9D9E-9E64AEDF6B54}"/>
     <hyperlink ref="H1" r:id="rId7" xr:uid="{5AEA8CA4-B61F-4219-9540-5D497AE6B054}"/>
+    <hyperlink ref="H7" r:id="rId8" display="aris@poltekedc.ac.id" xr:uid="{6A13F8F7-DE16-4CF1-9BAB-F07C7C2B5BC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>